<commit_message>
feat: use case of not existing student
</commit_message>
<xml_diff>
--- a/REGISTROS DE ASISTENCIA - SAAC (MARTES 31-12 INFORMATICA).xlsx
+++ b/REGISTROS DE ASISTENCIA - SAAC (MARTES 31-12 INFORMATICA).xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>FECHA</t>
   </si>
@@ -35,6 +35,24 @@
   </si>
   <si>
     <t>ASIGNATURA (Nombre de malla curricular) / NIVEL</t>
+  </si>
+  <si>
+    <t>31-12-2024</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>anadora</t>
+  </si>
+  <si>
+    <t>ana dora</t>
+  </si>
+  <si>
+    <t>FÍSICA MECANICA / 3</t>
   </si>
 </sst>
 </file>
@@ -396,7 +414,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -433,6 +451,29 @@
         <v>6</v>
       </c>
     </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fix: uppercase on db and on excel
</commit_message>
<xml_diff>
--- a/REGISTROS DE ASISTENCIA - SAAC (MARTES 31-12 INFORMATICA).xlsx
+++ b/REGISTROS DE ASISTENCIA - SAAC (MARTES 31-12 INFORMATICA).xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
   <si>
     <t>FECHA</t>
   </si>
@@ -40,19 +40,40 @@
     <t>31-12-2024</t>
   </si>
   <si>
-    <t>123</t>
+    <t>20357099</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>MATIAS IGNACIO</t>
+  </si>
+  <si>
+    <t>CEBALLOS VASQUEZ</t>
   </si>
   <si>
     <t>1</t>
   </si>
   <si>
-    <t>anadora</t>
-  </si>
-  <si>
-    <t>ana dora</t>
-  </si>
-  <si>
     <t>FÍSICA MECANICA / 3</t>
+  </si>
+  <si>
+    <t>21075353</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>FLAVIO ALEXANDER</t>
+  </si>
+  <si>
+    <t>JARA LABRIN</t>
+  </si>
+  <si>
+    <t>ANA DORA</t>
+  </si>
+  <si>
+    <t>LABRIN ESPINOZA</t>
   </si>
 </sst>
 </file>
@@ -414,7 +435,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -468,10 +489,56 @@
         <v>11</v>
       </c>
       <c r="F2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="G2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" t="s">
         <v>12</v>
+      </c>
+      <c r="G3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: added selection in case of 2+ students with the same name
</commit_message>
<xml_diff>
--- a/REGISTROS DE ASISTENCIA - SAAC (MARTES 31-12 INFORMATICA).xlsx
+++ b/REGISTROS DE ASISTENCIA - SAAC (MARTES 31-12 INFORMATICA).xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t>FECHA</t>
   </si>
@@ -40,6 +40,24 @@
     <t>31-12-2024</t>
   </si>
   <si>
+    <t>21494146</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>MAXIMILIANO JOAQUIN</t>
+  </si>
+  <si>
+    <t>ALMONACID PÉREZ</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>FÍSICA MECANICA / 3</t>
+  </si>
+  <si>
     <t>20357099</t>
   </si>
   <si>
@@ -50,30 +68,6 @@
   </si>
   <si>
     <t>CEBALLOS VASQUEZ</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>FÍSICA MECANICA / 3</t>
-  </si>
-  <si>
-    <t>21075353</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>FLAVIO ALEXANDER</t>
-  </si>
-  <si>
-    <t>JARA LABRIN</t>
-  </si>
-  <si>
-    <t>ANA DORA</t>
-  </si>
-  <si>
-    <t>LABRIN ESPINOZA</t>
   </si>
 </sst>
 </file>
@@ -435,7 +429,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -518,29 +512,6 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" t="s">
-        <v>13</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
feat: added coloring and spaces
</commit_message>
<xml_diff>
--- a/REGISTROS DE ASISTENCIA - SAAC (MARTES 31-12 INFORMATICA).xlsx
+++ b/REGISTROS DE ASISTENCIA - SAAC (MARTES 31-12 INFORMATICA).xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
   <si>
     <t>FECHA</t>
   </si>
@@ -40,6 +40,24 @@
     <t>31-12-2024</t>
   </si>
   <si>
+    <t>21075353</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>FLAVIO ALEXANDER</t>
+  </si>
+  <si>
+    <t>JARA LABRIN</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>FÍSICA MECANICA / 3</t>
+  </si>
+  <si>
     <t>21494146</t>
   </si>
   <si>
@@ -52,22 +70,16 @@
     <t>ALMONACID PÉREZ</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>FÍSICA MECANICA / 3</t>
-  </si>
-  <si>
-    <t>20357099</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>MATIAS IGNACIO</t>
-  </si>
-  <si>
-    <t>CEBALLOS VASQUEZ</t>
+    <t>21223313</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>MATHIAS EDUARDO</t>
+  </si>
+  <si>
+    <t>DEUMACÁN PULGAR</t>
   </si>
 </sst>
 </file>
@@ -429,7 +441,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -512,6 +524,29 @@
         <v>13</v>
       </c>
     </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fix: date formatting and border colors
</commit_message>
<xml_diff>
--- a/REGISTROS DE ASISTENCIA - SAAC (MARTES 31-12 INFORMATICA).xlsx
+++ b/REGISTROS DE ASISTENCIA - SAAC (MARTES 31-12 INFORMATICA).xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t>FECHA</t>
   </si>
@@ -37,7 +37,25 @@
     <t>ASIGNATURA (Nombre de malla curricular) / NIVEL</t>
   </si>
   <si>
-    <t>31-12-2024</t>
+    <t>31/12/2024</t>
+  </si>
+  <si>
+    <t>21494146</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>MAXIMILIANO JOAQUIN</t>
+  </si>
+  <si>
+    <t>ALMONACID PÉREZ</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>FÍSICA MECANICA / 3</t>
   </si>
   <si>
     <t>21075353</t>
@@ -50,36 +68,6 @@
   </si>
   <si>
     <t>JARA LABRIN</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>FÍSICA MECANICA / 3</t>
-  </si>
-  <si>
-    <t>21494146</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>MAXIMILIANO JOAQUIN</t>
-  </si>
-  <si>
-    <t>ALMONACID PÉREZ</t>
-  </si>
-  <si>
-    <t>21223313</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>MATHIAS EDUARDO</t>
-  </si>
-  <si>
-    <t>DEUMACÁN PULGAR</t>
   </si>
 </sst>
 </file>
@@ -144,9 +132,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -441,7 +430,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -479,71 +468,48 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="G3" s="2" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>